<commit_message>
Trial to Trial # rename
</commit_message>
<xml_diff>
--- a/docs/provided/SampleData.xlsx
+++ b/docs/provided/SampleData.xlsx
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="21">
   <si>
     <t xml:space="preserve">Horse ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Trial</t>
+    <t xml:space="preserve">Trial #</t>
   </si>
   <si>
     <t xml:space="preserve">Trial Start</t>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t xml:space="preserve">Trial type (pos/neg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trial #</t>
   </si>
   <si>
     <t xml:space="preserve">Start</t>
@@ -210,13 +207,14 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35:A44"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="25.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,7 +280,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="n">
@@ -332,7 +330,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="n">
@@ -382,7 +380,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="n">
@@ -432,7 +430,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="n">
@@ -482,7 +480,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="n">
@@ -544,7 +542,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="n">
@@ -594,7 +592,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B16" s="1" t="n">
@@ -644,7 +642,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B18" s="1" t="n">
@@ -694,7 +692,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B20" s="1" t="n">
@@ -744,7 +742,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B22" s="1" t="n">
@@ -806,7 +804,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B25" s="1" t="n">
@@ -856,7 +854,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B27" s="1" t="n">
@@ -906,7 +904,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B29" s="1" t="n">
@@ -956,7 +954,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B31" s="1" t="n">
@@ -1006,7 +1004,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B33" s="1" t="n">
@@ -1068,7 +1066,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B36" s="1" t="n">
@@ -1118,7 +1116,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B38" s="1" t="n">
@@ -1168,7 +1166,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B40" s="1" t="n">
@@ -1218,7 +1216,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B42" s="1" t="n">
@@ -1268,7 +1266,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B44" s="1" t="n">
@@ -1311,7 +1309,7 @@
   <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="A35:A44 L2"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1334,37 +1332,37 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
@@ -1395,7 +1393,7 @@
         <v>0.00277777777777777</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="5" t="n">
@@ -1420,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2</v>
@@ -1443,7 +1441,7 @@
         <v>0.00240740740740741</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -1452,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>3</v>
@@ -1475,7 +1473,7 @@
         <v>0.00328703703703704</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" s="2"/>
     </row>
@@ -1484,7 +1482,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>4</v>
@@ -1507,7 +1505,7 @@
         <v>0.00163194444444444</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" s="2"/>
     </row>
@@ -1516,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>5</v>
@@ -1539,7 +1537,7 @@
         <v>0.001875</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" s="2"/>
     </row>
@@ -1548,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>6</v>
@@ -1571,7 +1569,7 @@
         <v>0.00136574074074074</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="2"/>
     </row>
@@ -1580,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>7</v>
@@ -1603,7 +1601,7 @@
         <v>0.00287037037037037</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="2"/>
     </row>
@@ -1612,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>8</v>
@@ -1635,7 +1633,7 @@
         <v>0.00175925925925926</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" s="2"/>
     </row>
@@ -1644,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>9</v>
@@ -1667,7 +1665,7 @@
         <v>0.00211805555555556</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J10" s="2"/>
     </row>
@@ -1676,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>10</v>
@@ -1699,7 +1697,7 @@
         <v>0.00142361111111111</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J11" s="2"/>
     </row>
@@ -1708,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>1</v>
@@ -1731,7 +1729,7 @@
         <v>0.000381944444444444</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,7 +1737,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>2</v>
@@ -1762,7 +1760,7 @@
         <v>0.000208333333333333</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>3</v>
@@ -1793,7 +1791,7 @@
         <v>0.000509259259259259</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>4</v>
@@ -1824,7 +1822,7 @@
         <v>0.00131944444444444</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>5</v>
@@ -1855,7 +1853,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>6</v>
@@ -1886,7 +1884,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1892,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>7</v>
@@ -1917,7 +1915,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>8</v>
@@ -1948,7 +1946,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>9</v>
@@ -1979,7 +1977,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,7 +1985,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>10</v>
@@ -2010,7 +2008,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2018,7 +2016,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
@@ -2041,7 +2039,7 @@
         <v>0.00277777777777777</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2" t="n">
@@ -2066,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>2</v>
@@ -2089,7 +2087,7 @@
         <v>0.00240740740740741</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J24" s="2"/>
     </row>
@@ -2098,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>3</v>
@@ -2121,7 +2119,7 @@
         <v>0.00328703703703704</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J25" s="2"/>
     </row>
@@ -2130,7 +2128,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>4</v>
@@ -2153,7 +2151,7 @@
         <v>0.00163194444444444</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J26" s="2"/>
     </row>
@@ -2162,7 +2160,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>5</v>
@@ -2185,7 +2183,7 @@
         <v>0.001875</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J27" s="2"/>
     </row>
@@ -2194,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>6</v>
@@ -2217,7 +2215,7 @@
         <v>0.00149305555555556</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="4"/>
@@ -2229,7 +2227,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>7</v>
@@ -2252,7 +2250,7 @@
         <v>0.000810185185185185</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="4"/>
@@ -2264,7 +2262,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>8</v>
@@ -2287,7 +2285,7 @@
         <v>0.000763888888888889</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="4"/>
@@ -2299,7 +2297,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>9</v>
@@ -2322,7 +2320,7 @@
         <v>0.000625</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="4"/>
@@ -2334,7 +2332,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>10</v>
@@ -2357,7 +2355,7 @@
         <v>0.000821759259259259</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="4"/>
@@ -2369,7 +2367,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>1</v>
@@ -2392,7 +2390,7 @@
         <v>0.000381944444444444</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -2403,7 +2401,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>2</v>
@@ -2426,7 +2424,7 @@
         <v>0.000208333333333333</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -2437,7 +2435,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>3</v>
@@ -2460,7 +2458,7 @@
         <v>0.000509259259259259</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -2471,7 +2469,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>4</v>
@@ -2494,7 +2492,7 @@
         <v>0.00025462962962963</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -2505,7 +2503,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>5</v>
@@ -2528,7 +2526,7 @@
         <v>0.00056712962962963</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -2539,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>6</v>
@@ -2562,7 +2560,7 @@
         <v>0.000601851851851852</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -2573,7 +2571,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>7</v>
@@ -2596,7 +2594,7 @@
         <v>0.000844907407407407</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
@@ -2607,7 +2605,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>8</v>
@@ -2630,7 +2628,7 @@
         <v>0.000243055555555556</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
@@ -2641,7 +2639,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>9</v>
@@ -2664,7 +2662,7 @@
         <v>0.00167824074074074</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
@@ -2675,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>10</v>
@@ -2698,7 +2696,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
@@ -2709,7 +2707,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>1</v>
@@ -2732,7 +2730,7 @@
         <v>0.00277777777777777</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K44" s="2" t="n">
         <f aca="false">AVERAGE(G44:G63)</f>
@@ -2756,7 +2754,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>2</v>
@@ -2779,7 +2777,7 @@
         <v>0.00240740740740741</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2787,7 +2785,7 @@
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>3</v>
@@ -2810,7 +2808,7 @@
         <v>0.00328703703703704</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,7 +2816,7 @@
         <v>3</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>4</v>
@@ -2841,7 +2839,7 @@
         <v>0.00246527777777778</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2849,7 +2847,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>5</v>
@@ -2872,7 +2870,7 @@
         <v>0.00206018518518519</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>6</v>
@@ -2903,7 +2901,7 @@
         <v>0.00167824074074074</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2911,7 +2909,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>7</v>
@@ -2934,7 +2932,7 @@
         <v>0.0019212962962963</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2942,7 +2940,7 @@
         <v>3</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>8</v>
@@ -2965,7 +2963,7 @@
         <v>0.0015625</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2973,7 +2971,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>9</v>
@@ -2996,7 +2994,7 @@
         <v>0.00125</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3004,7 +3002,7 @@
         <v>3</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>10</v>
@@ -3027,7 +3025,7 @@
         <v>0.00099537037037037</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3035,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>1</v>
@@ -3058,7 +3056,7 @@
         <v>0.00025462962962963</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3066,7 +3064,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>2</v>
@@ -3089,7 +3087,7 @@
         <v>0.000243055555555556</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,7 +3095,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>3</v>
@@ -3120,7 +3118,7 @@
         <v>0.000706018518518519</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3128,7 +3126,7 @@
         <v>3</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>4</v>
@@ -3151,7 +3149,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,7 +3157,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>5</v>
@@ -3182,7 +3180,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3190,7 +3188,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>6</v>
@@ -3213,7 +3211,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3221,7 +3219,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>7</v>
@@ -3244,7 +3242,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,7 +3250,7 @@
         <v>3</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>8</v>
@@ -3275,7 +3273,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3283,7 +3281,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>9</v>
@@ -3306,7 +3304,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3314,7 +3312,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>10</v>
@@ -3337,7 +3335,7 @@
         <v>0.000347222222222222</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>